<commit_message>
setup admin data loaders
</commit_message>
<xml_diff>
--- a/input_data/admin_data/BRA/_clean/total-pre-BRA.xlsx
+++ b/input_data/admin_data/BRA/_clean/total-pre-BRA.xlsx
@@ -269,10 +269,10 @@
         <v>1.016E8</v>
       </c>
       <c r="F2" t="n">
-        <v>5195.588416428523</v>
+        <v>50.78894822397268</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9388370513916016</v>
+        <v>0.9994021058082581</v>
       </c>
       <c r="H2" t="n">
         <v>10694.442201712676</v>
@@ -295,7 +295,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9449533820152283</v>
+        <v>0.9994618892669678</v>
       </c>
       <c r="H3" t="n">
         <v>12411.203215735903</v>
@@ -318,7 +318,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9510696530342102</v>
+        <v>0.9995216727256775</v>
       </c>
       <c r="H4" t="n">
         <v>14073.222551913332</v>
@@ -341,7 +341,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9571859240531921</v>
+        <v>0.9995814561843872</v>
       </c>
       <c r="H5" t="n">
         <v>15293.406232014124</v>
@@ -364,7 +364,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9633022546768188</v>
+        <v>0.9996412396430969</v>
       </c>
       <c r="H6" t="n">
         <v>16840.34806997287</v>
@@ -387,7 +387,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9694185256958008</v>
+        <v>0.9997010827064514</v>
       </c>
       <c r="H7" t="n">
         <v>20828.442914136063</v>
@@ -410,7 +410,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9755348563194275</v>
+        <v>0.9997608661651611</v>
       </c>
       <c r="H8" t="n">
         <v>25568.133954782967</v>
@@ -433,7 +433,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9816511273384094</v>
+        <v>0.9998206496238708</v>
       </c>
       <c r="H9" t="n">
         <v>31763.745782599497</v>
@@ -456,7 +456,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9877673983573914</v>
+        <v>0.9998804330825806</v>
       </c>
       <c r="H10" t="n">
         <v>44744.872346749515</v>
@@ -479,7 +479,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9938837289810181</v>
+        <v>0.9999402165412903</v>
       </c>
       <c r="H11" t="n">
         <v>67085.93743417204</v>
@@ -502,7 +502,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9944953322410583</v>
+        <v>0.9999461770057678</v>
       </c>
       <c r="H12" t="n">
         <v>72134.19710727516</v>
@@ -525,7 +525,7 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.9951069951057434</v>
+        <v>0.9999521970748901</v>
       </c>
       <c r="H13" t="n">
         <v>78338.67185895971</v>
@@ -548,7 +548,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.9957185983657837</v>
+        <v>0.9999581575393677</v>
       </c>
       <c r="H14" t="n">
         <v>85242.52080843282</v>
@@ -571,7 +571,7 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.996330201625824</v>
+        <v>0.9999641180038452</v>
       </c>
       <c r="H15" t="n">
         <v>92289.77700174361</v>
@@ -594,7 +594,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.996941864490509</v>
+        <v>0.9999700784683228</v>
       </c>
       <c r="H16" t="n">
         <v>99773.16393188074</v>
@@ -617,7 +617,7 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>0.9975534677505493</v>
+        <v>0.9999760985374451</v>
       </c>
       <c r="H17" t="n">
         <v>109481.3935522444</v>
@@ -640,7 +640,7 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>0.9981651306152344</v>
+        <v>0.9999820590019226</v>
       </c>
       <c r="H18" t="n">
         <v>125989.00518741626</v>
@@ -663,7 +663,7 @@
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19" t="n">
-        <v>0.9987767338752747</v>
+        <v>0.9999880194664001</v>
       </c>
       <c r="H19" t="n">
         <v>157968.74260545315</v>
@@ -686,7 +686,7 @@
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>0.9993883967399597</v>
+        <v>0.9999940395355225</v>
       </c>
       <c r="H20" t="n">
         <v>192400.5689980001</v>
@@ -709,7 +709,7 @@
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>0.9994495511054993</v>
+        <v>0.9999946355819702</v>
       </c>
       <c r="H21" t="n">
         <v>204703.8932905606</v>
@@ -732,7 +732,7 @@
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>0.9995107054710388</v>
+        <v>0.999995231628418</v>
       </c>
       <c r="H22" t="n">
         <v>222474.33617299914</v>
@@ -755,7 +755,7 @@
       <c r="E23"/>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>0.9995718598365784</v>
+        <v>0.9999958276748657</v>
       </c>
       <c r="H23" t="n">
         <v>237381.99415824402</v>
@@ -778,7 +778,7 @@
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>0.9996330142021179</v>
+        <v>0.9999964237213135</v>
       </c>
       <c r="H24" t="n">
         <v>252240.3318968395</v>
@@ -801,7 +801,7 @@
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>0.9996941685676575</v>
+        <v>0.9999970197677612</v>
       </c>
       <c r="H25" t="n">
         <v>274151.05868132703</v>
@@ -824,7 +824,7 @@
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="n">
-        <v>0.999755322933197</v>
+        <v>0.999997615814209</v>
       </c>
       <c r="H26" t="n">
         <v>311704.76856319094</v>
@@ -847,7 +847,7 @@
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="n">
-        <v>0.9998165369033813</v>
+        <v>0.9999982118606567</v>
       </c>
       <c r="H27" t="n">
         <v>384600.9979788212</v>
@@ -870,7 +870,7 @@
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>0.9998776912689209</v>
+        <v>0.9999988079071045</v>
       </c>
       <c r="H28" t="n">
         <v>535965.8381845559</v>
@@ -893,7 +893,7 @@
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>0.9999388456344604</v>
+        <v>0.9999994039535522</v>
       </c>
       <c r="H29" t="n">
         <v>998180.3788071432</v>
@@ -916,7 +916,7 @@
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>0.9999449253082275</v>
+        <v>0.999999463558197</v>
       </c>
       <c r="H30" t="n">
         <v>1105430.479452539</v>
@@ -939,7 +939,7 @@
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="n">
-        <v>0.9999510645866394</v>
+        <v>0.9999995231628418</v>
       </c>
       <c r="H31" t="n">
         <v>1241756.7883425585</v>
@@ -962,7 +962,7 @@
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>0.9999572038650513</v>
+        <v>0.9999995827674866</v>
       </c>
       <c r="H32" t="n">
         <v>1417085.0293154533</v>
@@ -985,7 +985,7 @@
       <c r="E33"/>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>0.9999632835388184</v>
+        <v>0.9999996423721313</v>
       </c>
       <c r="H33" t="n">
         <v>1648260.1972928615</v>
@@ -1008,7 +1008,7 @@
       <c r="E34"/>
       <c r="F34"/>
       <c r="G34" t="n">
-        <v>0.9999694228172302</v>
+        <v>0.9999997019767761</v>
       </c>
       <c r="H34" t="n">
         <v>1968701.0777093547</v>
@@ -1031,7 +1031,7 @@
       <c r="E35"/>
       <c r="F35"/>
       <c r="G35" t="n">
-        <v>0.9999755620956421</v>
+        <v>0.9999997615814209</v>
       </c>
       <c r="H35" t="n">
         <v>2452454.157007665</v>
@@ -1054,7 +1054,7 @@
       <c r="E36"/>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>0.9999816417694092</v>
+        <v>0.9999998211860657</v>
       </c>
       <c r="H36" t="n">
         <v>3261094.286644589</v>
@@ -1077,7 +1077,7 @@
       <c r="E37"/>
       <c r="F37"/>
       <c r="G37" t="n">
-        <v>0.999987781047821</v>
+        <v>0.9999998807907104</v>
       </c>
       <c r="H37" t="n">
         <v>4750284.772700311</v>
@@ -1100,7 +1100,7 @@
       <c r="E38"/>
       <c r="F38"/>
       <c r="G38" t="n">
-        <v>0.9999938607215881</v>
+        <v>0.9999999403953552</v>
       </c>
       <c r="H38" t="n">
         <v>8230911.2459120415</v>
@@ -1163,13 +1163,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>2.01467084E8</v>
+        <v>1.98478299E8</v>
       </c>
       <c r="F2" t="n">
-        <v>10501.207262969221</v>
+        <v>10659.339667910142</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8684925821430959</v>
+        <v>0.8665122779997223</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -1192,7 +1192,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8747898291911547</v>
+        <v>0.8729043521276852</v>
       </c>
       <c r="H3" t="n">
         <v>4068.0</v>
@@ -1215,7 +1215,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8773626613864128</v>
+        <v>0.8755159273105217</v>
       </c>
       <c r="H4" t="n">
         <v>8136.0</v>
@@ -1238,7 +1238,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8827026255068049</v>
+        <v>0.8809363032680968</v>
       </c>
       <c r="H5" t="n">
         <v>16272.0</v>
@@ -1261,7 +1261,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8960691514252521</v>
+        <v>0.8945041089857385</v>
       </c>
       <c r="H6" t="n">
         <v>24408.0</v>
@@ -1284,7 +1284,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9351922967227738</v>
+        <v>0.9342163900749674</v>
       </c>
       <c r="H7" t="n">
         <v>40680.0</v>
@@ -1307,7 +1307,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9714283699068181</v>
+        <v>0.9709981240820691</v>
       </c>
       <c r="H8" t="n">
         <v>81360.0</v>
@@ -1330,7 +1330,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9889109974907861</v>
+        <v>0.9887440137725082</v>
       </c>
       <c r="H9" t="n">
         <v>162720.0</v>
@@ -1353,7 +1353,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9963928350697725</v>
+        <v>0.9963385165851305</v>
       </c>
       <c r="H10" t="n">
         <v>325440.0</v>
@@ -1376,7 +1376,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9989667890363668</v>
+        <v>0.9989512304314941</v>
       </c>
       <c r="H11" t="n">
         <v>650880.0</v>
@@ -1399,7 +1399,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.999645401131631</v>
+        <v>0.9996400614054033</v>
       </c>
       <c r="H12" t="n">
         <v>1301760.0</v>
@@ -1462,13 +1462,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>2.03190852E8</v>
+        <v>2.00085127E8</v>
       </c>
       <c r="F2" t="n">
-        <v>11723.118935020217</v>
+        <v>11905.085401495586</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8642602128564332</v>
+        <v>0.8621532573982873</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -1491,7 +1491,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8700350250020115</v>
+        <v>0.868017706283586</v>
       </c>
       <c r="H3" t="n">
         <v>4344.0</v>
@@ -1514,7 +1514,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8725033989227035</v>
+        <v>0.8705243943494111</v>
       </c>
       <c r="H4" t="n">
         <v>8688.0</v>
@@ -1537,7 +1537,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8777566669192371</v>
+        <v>0.8758592036678469</v>
       </c>
       <c r="H5" t="n">
         <v>17376.0</v>
@@ -1560,7 +1560,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8912651736900045</v>
+        <v>0.8895773897277233</v>
       </c>
       <c r="H6" t="n">
         <v>26064.0</v>
@@ -1583,7 +1583,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9315847152410188</v>
+        <v>0.9305227719399654</v>
       </c>
       <c r="H7" t="n">
         <v>43440.0</v>
@@ -1606,7 +1606,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9532219787138843</v>
+        <v>0.95249588941211</v>
       </c>
       <c r="H8" t="n">
         <v>60816.0</v>
@@ -1629,7 +1629,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9699736629875444</v>
+        <v>0.969507593635383</v>
       </c>
       <c r="H9" t="n">
         <v>86880.0</v>
@@ -1652,7 +1652,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9825906434016035</v>
+        <v>0.9823204150501401</v>
       </c>
       <c r="H10" t="n">
         <v>130320.0</v>
@@ -1675,7 +1675,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9884340609979824</v>
+        <v>0.9882545342813012</v>
       </c>
       <c r="H11" t="n">
         <v>173760.0</v>
@@ -1698,7 +1698,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9937865755885507</v>
+        <v>0.993690130701219</v>
       </c>
       <c r="H12" t="n">
         <v>260640.0</v>
@@ -1721,7 +1721,7 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.9962558107684887</v>
+        <v>0.9961976933947719</v>
       </c>
       <c r="H13" t="n">
         <v>347520.0</v>
@@ -1744,7 +1744,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.998226514646437</v>
+        <v>0.9981989865743495</v>
       </c>
       <c r="H14" t="n">
         <v>521280.0</v>
@@ -1767,7 +1767,7 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.9989334854504178</v>
+        <v>0.9989169309920772</v>
       </c>
       <c r="H15" t="n">
         <v>695040.0</v>
@@ -1790,7 +1790,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.9996328033508123</v>
+        <v>0.9996271037177091</v>
       </c>
       <c r="H16" t="n">
         <v>1390080.0</v>
@@ -1813,7 +1813,7 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>0.9997933716031665</v>
+        <v>0.9997901643134125</v>
       </c>
       <c r="H17" t="n">
         <v>2085120.0</v>
@@ -1836,7 +1836,7 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>0.9998600675191814</v>
+        <v>0.9998578954846554</v>
       </c>
       <c r="H18" t="n">
         <v>2780160.0</v>
@@ -1899,13 +1899,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>2.04860101E8</v>
+        <v>2.01675532E8</v>
       </c>
       <c r="F2" t="n">
-        <v>12536.361726173463</v>
+        <v>12734.317861605692</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8656700652510173</v>
+        <v>0.8635489207486012</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -1928,7 +1928,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8720225272172447</v>
+        <v>0.8700016916281148</v>
       </c>
       <c r="H3" t="n">
         <v>4728.0</v>
@@ -1951,7 +1951,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8748228480078705</v>
+        <v>0.8728462310440317</v>
       </c>
       <c r="H4" t="n">
         <v>9456.0</v>
@@ -1974,7 +1974,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8808136094787926</v>
+        <v>0.8789315899759224</v>
       </c>
       <c r="H5" t="n">
         <v>18912.0</v>
@@ -1997,7 +1997,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8968149439699827</v>
+        <v>0.8951855944527768</v>
       </c>
       <c r="H6" t="n">
         <v>28368.0</v>
@@ -2020,7 +2020,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9329560371543505</v>
+        <v>0.9318973756320623</v>
       </c>
       <c r="H7" t="n">
         <v>47280.0</v>
@@ -2043,7 +2043,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9541398009952168</v>
+        <v>0.95341564290506</v>
       </c>
       <c r="H8" t="n">
         <v>66192.0</v>
@@ -2066,7 +2066,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9705043833791726</v>
+        <v>0.9700386311612655</v>
       </c>
       <c r="H9" t="n">
         <v>94560.0</v>
@@ -2089,7 +2089,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9828852813071688</v>
+        <v>0.9826150303647148</v>
       </c>
       <c r="H10" t="n">
         <v>141840.0</v>
@@ -2112,7 +2112,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9886478480258096</v>
+        <v>0.9884685912220625</v>
       </c>
       <c r="H11" t="n">
         <v>189120.0</v>
@@ -2135,7 +2135,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9939520092299476</v>
+        <v>0.9938565080864643</v>
       </c>
       <c r="H12" t="n">
         <v>283680.0</v>
@@ -2158,7 +2158,7 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.9963410591113592</v>
+        <v>0.996283282396399</v>
       </c>
       <c r="H13" t="n">
         <v>378240.0</v>
@@ -2181,7 +2181,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.9982438747308828</v>
+        <v>0.9982161445345784</v>
       </c>
       <c r="H14" t="n">
         <v>567360.0</v>
@@ -2204,7 +2204,7 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.9989415020350888</v>
+        <v>0.9989247877625532</v>
       </c>
       <c r="H15" t="n">
         <v>756480.0</v>
@@ -2227,7 +2227,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.9996319781175935</v>
+        <v>0.9996261668470521</v>
       </c>
       <c r="H16" t="n">
         <v>1512960.0</v>
@@ -2250,7 +2250,7 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>0.999789788251642</v>
+        <v>0.9997864688910304</v>
       </c>
       <c r="H17" t="n">
         <v>2269440.0</v>
@@ -2273,7 +2273,7 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>0.9998569218707941</v>
+        <v>0.9998546625874278</v>
       </c>
       <c r="H18" t="n">
         <v>3025920.0</v>
@@ -2336,13 +2336,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>2.04532726E8</v>
+        <v>2.03218114E8</v>
       </c>
       <c r="F2" t="n">
-        <v>13336.089036470183</v>
+        <v>13422.359804047586</v>
       </c>
       <c r="G2" t="n">
-        <v>0.863084761311009</v>
+        <v>0.8621990606605079</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -2365,7 +2365,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8694608949767775</v>
+        <v>0.8686164413473496</v>
       </c>
       <c r="H3" t="n">
         <v>5280.0</v>
@@ -2388,7 +2388,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8723370752903377</v>
+        <v>0.8715112275867298</v>
       </c>
       <c r="H4" t="n">
         <v>10560.0</v>
@@ -2411,7 +2411,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8789868375391428</v>
+        <v>0.8782040069518606</v>
       </c>
       <c r="H5" t="n">
         <v>21120.0</v>
@@ -2434,7 +2434,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8985150229699672</v>
+        <v>0.897858519639642</v>
       </c>
       <c r="H6" t="n">
         <v>31680.0</v>
@@ -2457,7 +2457,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9357006369728823</v>
+        <v>0.9352846862853967</v>
       </c>
       <c r="H7" t="n">
         <v>52800.0</v>
@@ -2480,7 +2480,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9563283872723625</v>
+        <v>0.9560458768946158</v>
       </c>
       <c r="H8" t="n">
         <v>73920.0</v>
@@ -2503,7 +2503,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9719866785523603</v>
+        <v>0.9718054612001763</v>
       </c>
       <c r="H9" t="n">
         <v>105600.0</v>
@@ -2526,7 +2526,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9839217319188324</v>
+        <v>0.9838177220757004</v>
       </c>
       <c r="H10" t="n">
         <v>158400.0</v>
@@ -2549,7 +2549,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9894026983241792</v>
+        <v>0.9893341446914521</v>
       </c>
       <c r="H11" t="n">
         <v>211200.0</v>
@@ -2572,7 +2572,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9944802134011552</v>
+        <v>0.9944445060640608</v>
       </c>
       <c r="H12" t="n">
         <v>316800.0</v>
@@ -2595,7 +2595,7 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.9966790448976854</v>
+        <v>0.9966575617368439</v>
       </c>
       <c r="H13" t="n">
         <v>422400.0</v>
@@ -2618,7 +2618,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.9984117798341963</v>
+        <v>0.9984015056846753</v>
       </c>
       <c r="H14" t="n">
         <v>633600.0</v>
@@ -2641,7 +2641,7 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.9990374792149399</v>
+        <v>0.9990312526963024</v>
       </c>
       <c r="H15" t="n">
         <v>844800.0</v>
@@ -2664,7 +2664,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.9996678575535144</v>
+        <v>0.999665708933801</v>
       </c>
       <c r="H16" t="n">
         <v>1689600.0</v>
@@ -2687,7 +2687,7 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>0.9998121571997236</v>
+        <v>0.9998109420501757</v>
       </c>
       <c r="H17" t="n">
         <v>2534400.0</v>
@@ -2710,7 +2710,7 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>0.9998739321549941</v>
+        <v>0.9998731166258141</v>
       </c>
       <c r="H18" t="n">
         <v>3379200.0</v>
@@ -2773,13 +2773,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>2.06172275E8</v>
+        <v>2.04703445E8</v>
       </c>
       <c r="F2" t="n">
-        <v>14174.970822520681</v>
+        <v>14276.681970534057</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8588485478952007</v>
+        <v>0.8578357291446659</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -2802,7 +2802,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8654053654886429</v>
+        <v>0.8644395945559197</v>
       </c>
       <c r="H3" t="n">
         <v>5622.0</v>
@@ -2825,7 +2825,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8685132954952357</v>
+        <v>0.8675698252171574</v>
       </c>
       <c r="H4" t="n">
         <v>11244.0</v>
@@ -2848,7 +2848,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8761711195164336</v>
+        <v>0.8752825972225333</v>
       </c>
       <c r="H5" t="n">
         <v>22488.0</v>
@@ -2871,7 +2871,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.897694217129825</v>
+        <v>0.896960131765247</v>
       </c>
       <c r="H6" t="n">
         <v>33732.0</v>
@@ -2894,7 +2894,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9362321388751228</v>
+        <v>0.9357745786838125</v>
       </c>
       <c r="H7" t="n">
         <v>56220.0</v>
@@ -2917,7 +2917,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9567046199592064</v>
+        <v>0.956393958098751</v>
       </c>
       <c r="H8" t="n">
         <v>78708.0</v>
@@ -2940,7 +2940,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9721901599038959</v>
+        <v>0.9719906130549</v>
       </c>
       <c r="H9" t="n">
         <v>112440.0</v>
@@ -2963,7 +2963,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9839731894116219</v>
+        <v>0.983858190564404</v>
       </c>
       <c r="H10" t="n">
         <v>168660.0</v>
@@ -2986,7 +2986,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9894455304429269</v>
+        <v>0.9893697978556247</v>
       </c>
       <c r="H11" t="n">
         <v>224880.0</v>
@@ -3009,7 +3009,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9944753095439239</v>
+        <v>0.9944356676557153</v>
       </c>
       <c r="H12" t="n">
         <v>337320.0</v>
@@ -3032,7 +3032,7 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.9967377863973224</v>
+        <v>0.9967143786954831</v>
       </c>
       <c r="H13" t="n">
         <v>449760.0</v>
@@ -3055,7 +3055,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.9984470365862723</v>
+        <v>0.99843589344576</v>
       </c>
       <c r="H14" t="n">
         <v>674640.0</v>
@@ -3078,7 +3078,7 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.9990577394559962</v>
+        <v>0.9990509783555426</v>
       </c>
       <c r="H15" t="n">
         <v>899520.0</v>
@@ -3101,7 +3101,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.9996741171915574</v>
+        <v>0.9996717788506198</v>
       </c>
       <c r="H16" t="n">
         <v>1799040.0</v>
@@ -3124,7 +3124,7 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>0.9998164302159445</v>
+        <v>0.9998151130285081</v>
       </c>
       <c r="H17" t="n">
         <v>2698560.0</v>
@@ -3147,7 +3147,7 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>0.9998778836776187</v>
+        <v>0.9998770074436216</v>
       </c>
       <c r="H18" t="n">
         <v>3598080.0</v>
@@ -3210,13 +3210,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>2.0785333E8</v>
+        <v>2.06107261E8</v>
       </c>
       <c r="F2" t="n">
-        <v>14812.350801969782</v>
+        <v>14937.835883994354</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8543732063373726</v>
+        <v>0.8531395068124261</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -3239,7 +3239,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8609599470934625</v>
+        <v>0.8597820481443398</v>
       </c>
       <c r="H3" t="n">
         <v>5724.0</v>
@@ -3262,7 +3262,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.863962155429504</v>
+        <v>0.8628096901447834</v>
       </c>
       <c r="H4" t="n">
         <v>11448.0</v>
@@ -3285,7 +3285,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8720436425050299</v>
+        <v>0.870959640766853</v>
       </c>
       <c r="H5" t="n">
         <v>22896.0</v>
@@ -3308,7 +3308,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8944637740468243</v>
+        <v>0.8935697078619661</v>
       </c>
       <c r="H6" t="n">
         <v>34344.0</v>
@@ -3331,7 +3331,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9343482108273176</v>
+        <v>0.9337920317130409</v>
       </c>
       <c r="H7" t="n">
         <v>57240.0</v>
@@ -3354,7 +3354,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9554720484872674</v>
+        <v>0.9550948231755891</v>
       </c>
       <c r="H8" t="n">
         <v>80136.0</v>
@@ -3377,7 +3377,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9713814784684951</v>
+        <v>0.9711390323119184</v>
       </c>
       <c r="H9" t="n">
         <v>114480.0</v>
@@ -3400,7 +3400,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9836087879852586</v>
+        <v>0.9834699273404055</v>
       </c>
       <c r="H10" t="n">
         <v>171720.0</v>
@@ -3423,7 +3423,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9892353420558622</v>
+        <v>0.9891441476193311</v>
       </c>
       <c r="H11" t="n">
         <v>228960.0</v>
@@ -3446,7 +3446,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9944099139523047</v>
+        <v>0.9943625566883837</v>
       </c>
       <c r="H12" t="n">
         <v>343440.0</v>
@@ -3469,7 +3469,7 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.9967547116036101</v>
+        <v>0.9967272186495166</v>
       </c>
       <c r="H13" t="n">
         <v>457920.0</v>
@@ -3492,7 +3492,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.9984713595880326</v>
+        <v>0.9984584094783541</v>
       </c>
       <c r="H14" t="n">
         <v>686880.0</v>
@@ -3515,7 +3515,7 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.9990656007291295</v>
+        <v>0.9990576848236317</v>
       </c>
       <c r="H15" t="n">
         <v>915840.0</v>
@@ -3538,7 +3538,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.9996696420499974</v>
+        <v>0.9996668433723934</v>
       </c>
       <c r="H16" t="n">
         <v>1831680.0</v>
@@ -3561,7 +3561,7 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>0.9998127958787093</v>
+        <v>0.9998112099505315</v>
       </c>
       <c r="H17" t="n">
         <v>2747520.0</v>
@@ -3584,7 +3584,7 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>0.999874435497377</v>
+        <v>0.999873371758601</v>
       </c>
       <c r="H18" t="n">
         <v>3663360.0</v>
@@ -3647,13 +3647,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>2.09496612E8</v>
+        <v>2.07455459E8</v>
       </c>
       <c r="F2" t="n">
-        <v>15806.532434192395</v>
+        <v>15962.052810726083</v>
       </c>
       <c r="G2" t="n">
-        <v>0.854419998925806</v>
+        <v>0.8529876381802033</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -3676,7 +3676,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8607543066137986</v>
+        <v>0.8593842690830324</v>
       </c>
       <c r="H3" t="n">
         <v>5988.0</v>
@@ -3699,7 +3699,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8626536690722235</v>
+        <v>0.8613023193571396</v>
       </c>
       <c r="H4" t="n">
         <v>11976.0</v>
@@ -3722,7 +3722,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8718539658292899</v>
+        <v>0.8705931377780712</v>
       </c>
       <c r="H5" t="n">
         <v>23952.0</v>
@@ -3745,7 +3745,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8954996847395318</v>
+        <v>0.894471506772931</v>
       </c>
       <c r="H6" t="n">
         <v>35928.0</v>
@@ -3768,7 +3768,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9349274297571935</v>
+        <v>0.9342871811341441</v>
       </c>
       <c r="H7" t="n">
         <v>59880.0</v>
@@ -3791,7 +3791,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9558477394374282</v>
+        <v>0.9554133256141503</v>
       </c>
       <c r="H8" t="n">
         <v>83832.0</v>
@@ -3814,7 +3814,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9714792189574885</v>
+        <v>0.9711986031661861</v>
       </c>
       <c r="H9" t="n">
         <v>119760.0</v>
@@ -3837,7 +3837,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9836319930558113</v>
+        <v>0.9834709483349869</v>
       </c>
       <c r="H10" t="n">
         <v>179640.0</v>
@@ -3860,7 +3860,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9892524705841066</v>
+        <v>0.9891467257075168</v>
       </c>
       <c r="H11" t="n">
         <v>239520.0</v>
@@ -3883,7 +3883,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.994446229994402</v>
+        <v>0.9943915864850777</v>
       </c>
       <c r="H12" t="n">
         <v>359280.0</v>
@@ -3906,7 +3906,7 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.9967355080663548</v>
+        <v>0.9967033887500641</v>
       </c>
       <c r="H13" t="n">
         <v>479040.0</v>
@@ -3929,7 +3929,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.9984679513576096</v>
+        <v>0.9984528775403302</v>
       </c>
       <c r="H14" t="n">
         <v>718560.0</v>
@@ -3952,7 +3952,7 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.9990690827973867</v>
+        <v>0.9990599235086891</v>
       </c>
       <c r="H15" t="n">
         <v>958080.0</v>
@@ -3975,7 +3975,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.9996713741604566</v>
+        <v>0.999668140812819</v>
       </c>
       <c r="H16" t="n">
         <v>1916160.0</v>
@@ -3998,7 +3998,7 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>0.9998129850424502</v>
+        <v>0.9998111450034197</v>
       </c>
       <c r="H17" t="n">
         <v>2874240.0</v>
@@ -4021,7 +4021,7 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>0.9998751196988331</v>
+        <v>0.9998738910023091</v>
       </c>
       <c r="H18" t="n">
         <v>3832320.0</v>
@@ -4084,13 +4084,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>2.11096328E8</v>
+        <v>2.08660842E8</v>
       </c>
       <c r="F2" t="n">
-        <v>16032.919715816799</v>
+        <v>16220.055697502314</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8501402497157601</v>
+        <v>0.8483910891148422</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -4113,7 +4113,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8577398418792013</v>
+        <v>0.8560793835960846</v>
       </c>
       <c r="H3" t="n">
         <v>6270.0</v>
@@ -4136,7 +4136,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8604797332144972</v>
+        <v>0.8588512548990864</v>
       </c>
       <c r="H4" t="n">
         <v>12540.0</v>
@@ -4159,7 +4159,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8735318077157648</v>
+        <v>0.8720556730045209</v>
       </c>
       <c r="H5" t="n">
         <v>25080.0</v>
@@ -4182,7 +4182,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8972880001967632</v>
+        <v>0.8960891473830054</v>
       </c>
       <c r="H6" t="n">
         <v>37620.0</v>
@@ -4205,7 +4205,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9364310875175432</v>
+        <v>0.9356891121909687</v>
       </c>
       <c r="H7" t="n">
         <v>62700.0</v>
@@ -4228,7 +4228,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9568810405835197</v>
+        <v>0.9563777567810255</v>
       </c>
       <c r="H8" t="n">
         <v>87780.0</v>
@@ -4251,7 +4251,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9721306852860084</v>
+        <v>0.9718053950918112</v>
       </c>
       <c r="H9" t="n">
         <v>125400.0</v>
@@ -4274,7 +4274,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.984097681699134</v>
+        <v>0.9839120700950684</v>
       </c>
       <c r="H10" t="n">
         <v>188100.0</v>
@@ -4297,7 +4297,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9896268636183951</v>
+        <v>0.989505788536979</v>
       </c>
       <c r="H11" t="n">
         <v>250800.0</v>
@@ -4320,7 +4320,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9947139677389367</v>
+        <v>0.9946522692551965</v>
       </c>
       <c r="H12" t="n">
         <v>376200.0</v>
@@ -4343,7 +4343,7 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.9969028547005327</v>
+        <v>0.9968667048702889</v>
       </c>
       <c r="H13" t="n">
         <v>501600.0</v>
@@ -4366,7 +4366,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.9985174351303733</v>
+        <v>0.9985001306570017</v>
       </c>
       <c r="H14" t="n">
         <v>752400.0</v>
@@ -4389,7 +4389,7 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.9990763600587121</v>
+        <v>0.9990655793481367</v>
       </c>
       <c r="H15" t="n">
         <v>1003200.0</v>
@@ -4412,7 +4412,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.9996573317940424</v>
+        <v>0.9996533321762403</v>
       </c>
       <c r="H16" t="n">
         <v>2006400.0</v>
@@ -4435,7 +4435,7 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>0.9998030567353119</v>
+        <v>0.9998007580166862</v>
       </c>
       <c r="H17" t="n">
         <v>3009600.0</v>
@@ -4458,7 +4458,7 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>0.9998673259726242</v>
+        <v>0.9998657774035054</v>
       </c>
       <c r="H18" t="n">
         <v>4012800.0</v>
@@ -4521,13 +4521,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>2.1265057E8</v>
+        <v>2.09550294E8</v>
       </c>
       <c r="F2" t="n">
-        <v>19822.994718040773</v>
+        <v>20116.273976205255</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8307408204925103</v>
+        <v>0.8282366475706304</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -4550,7 +4550,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8392365513057407</v>
+        <v>0.8368580718860743</v>
       </c>
       <c r="H3" t="n">
         <v>6600.0</v>
@@ -4573,7 +4573,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8441765850898024</v>
+        <v>0.8418711929843439</v>
       </c>
       <c r="H4" t="n">
         <v>13200.0</v>
@@ -4596,7 +4596,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8622661627476474</v>
+        <v>0.8602284041653504</v>
       </c>
       <c r="H5" t="n">
         <v>26400.0</v>
@@ -4619,7 +4619,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8976896041237981</v>
+        <v>0.8961759318743786</v>
       </c>
       <c r="H6" t="n">
         <v>39600.0</v>
@@ -4642,7 +4642,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9392082137376825</v>
+        <v>0.9383088052360355</v>
       </c>
       <c r="H7" t="n">
         <v>66000.0</v>
@@ -4665,7 +4665,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9590421177803568</v>
+        <v>0.95843614993926</v>
       </c>
       <c r="H8" t="n">
         <v>92400.0</v>
@@ -4688,7 +4688,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9736186928631322</v>
+        <v>0.9732283840174426</v>
       </c>
       <c r="H9" t="n">
         <v>132000.0</v>
@@ -4711,7 +4711,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9847495964859159</v>
+        <v>0.9845239682651078</v>
       </c>
       <c r="H10" t="n">
         <v>198000.0</v>
@@ -4734,7 +4734,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9899739464606184</v>
+        <v>0.9898256119841091</v>
       </c>
       <c r="H11" t="n">
         <v>264000.0</v>
@@ -4757,7 +4757,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9947448906438389</v>
+        <v>0.9946671418175151</v>
       </c>
       <c r="H12" t="n">
         <v>396000.0</v>
@@ -4780,7 +4780,7 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.9961574050800804</v>
+        <v>0.9961005542659844</v>
       </c>
       <c r="H13" t="n">
         <v>528000.0</v>
@@ -4803,7 +4803,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.9983316950431875</v>
+        <v>0.9983070126353533</v>
       </c>
       <c r="H14" t="n">
         <v>792000.0</v>
@@ -4826,7 +4826,7 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.9989181453875247</v>
+        <v>0.9989021394548843</v>
       </c>
       <c r="H15" t="n">
         <v>1056000.0</v>
@@ -4849,7 +4849,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.9995806829955829</v>
+        <v>0.9995744792417233</v>
       </c>
       <c r="H16" t="n">
         <v>2112000.0</v>
@@ -4872,7 +4872,7 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>0.9997495844944126</v>
+        <v>0.9997458796216244</v>
       </c>
       <c r="H17" t="n">
         <v>3168000.0</v>
@@ -4895,7 +4895,7 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>0.999833238161553</v>
+        <v>0.9998307709365466</v>
       </c>
       <c r="H18" t="n">
         <v>4224000.0</v>
@@ -4958,13 +4958,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>2.14152911E8</v>
+        <v>2.10306415E8</v>
       </c>
       <c r="F2" t="n">
-        <v>22691.463766349036</v>
+        <v>23106.489739814497</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8105572657847271</v>
+        <v>0.8070923656798581</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -4987,7 +4987,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8183514909120241</v>
+        <v>0.8150291468759999</v>
       </c>
       <c r="H3" t="n">
         <v>7272.0</v>
@@ -5010,7 +5010,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8212018607582692</v>
+        <v>0.8179316498738282</v>
       </c>
       <c r="H4" t="n">
         <v>14544.0</v>
@@ -5033,7 +5033,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8403404518745954</v>
+        <v>0.8374202850635821</v>
       </c>
       <c r="H5" t="n">
         <v>29088.0</v>
@@ -5056,7 +5056,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8812429544793813</v>
+        <v>0.8790708928208395</v>
       </c>
       <c r="H6" t="n">
         <v>43632.0</v>
@@ -5079,7 +5079,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9283119994572476</v>
+        <v>0.9270008287669209</v>
       </c>
       <c r="H7" t="n">
         <v>72720.0</v>
@@ -5102,7 +5102,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9515084714398302</v>
+        <v>0.9506215633032402</v>
       </c>
       <c r="H8" t="n">
         <v>101808.0</v>
@@ -5125,7 +5125,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9685957432537539</v>
+        <v>0.9680213606418044</v>
       </c>
       <c r="H9" t="n">
         <v>145440.0</v>
@@ -5148,7 +5148,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9818857190318557</v>
+        <v>0.9815544095504647</v>
       </c>
       <c r="H10" t="n">
         <v>218160.0</v>
@@ -5171,7 +5171,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9880517244054646</v>
+        <v>0.9878331909181182</v>
       </c>
       <c r="H11" t="n">
         <v>290880.0</v>
@@ -5194,7 +5194,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9936983158729978</v>
+        <v>0.9935830583199281</v>
       </c>
       <c r="H12" t="n">
         <v>436320.0</v>
@@ -5217,7 +5217,7 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.9961335991365534</v>
+        <v>0.9960628828179112</v>
       </c>
       <c r="H13" t="n">
         <v>581760.0</v>
@@ -5240,7 +5240,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.9979954556863343</v>
+        <v>0.9979587926502385</v>
       </c>
       <c r="H14" t="n">
         <v>872640.0</v>
@@ -5263,7 +5263,7 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.9987186118614096</v>
+        <v>0.9986951753231113</v>
       </c>
       <c r="H15" t="n">
         <v>1163520.0</v>
@@ -5286,7 +5286,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.9995169946580833</v>
+        <v>0.9995081605095117</v>
       </c>
       <c r="H16" t="n">
         <v>2327040.0</v>
@@ -5309,7 +5309,7 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>0.9997177951038919</v>
+        <v>0.9997126335875204</v>
       </c>
       <c r="H17" t="n">
         <v>3490560.0</v>
@@ -5332,7 +5332,7 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>0.9998085013189477</v>
+        <v>0.9998049988156567</v>
       </c>
       <c r="H18" t="n">
         <v>4654080.0</v>
@@ -5398,10 +5398,10 @@
         <v>1.067E8</v>
       </c>
       <c r="F2" t="n">
-        <v>6105.933366617469</v>
+        <v>60.14605058052778</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9378995895385742</v>
+        <v>0.9993882775306702</v>
       </c>
       <c r="H2" t="n">
         <v>13472.2</v>
@@ -5424,7 +5424,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.9441096186637878</v>
+        <v>0.9994494318962097</v>
       </c>
       <c r="H3" t="n">
         <v>14421.56</v>
@@ -5447,7 +5447,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.9503196477890015</v>
+        <v>0.999510645866394</v>
       </c>
       <c r="H4" t="n">
         <v>16190.85</v>
@@ -5470,7 +5470,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.9565296769142151</v>
+        <v>0.9995718002319336</v>
       </c>
       <c r="H5" t="n">
         <v>18458.85</v>
@@ -5493,7 +5493,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9627397656440735</v>
+        <v>0.9996329545974731</v>
       </c>
       <c r="H6" t="n">
         <v>21421.55</v>
@@ -5516,7 +5516,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9689497947692871</v>
+        <v>0.9996941685676575</v>
       </c>
       <c r="H7" t="n">
         <v>23898.59</v>
@@ -5539,7 +5539,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9751598238945007</v>
+        <v>0.999755322933197</v>
       </c>
       <c r="H8" t="n">
         <v>28527.67</v>
@@ -5562,7 +5562,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9813698530197144</v>
+        <v>0.9998164772987366</v>
       </c>
       <c r="H9" t="n">
         <v>37093.59</v>
@@ -5585,7 +5585,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9875799417495728</v>
+        <v>0.9998776316642761</v>
       </c>
       <c r="H10" t="n">
         <v>49473.6</v>
@@ -5608,7 +5608,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9937899708747864</v>
+        <v>0.9999388456344604</v>
       </c>
       <c r="H11" t="n">
         <v>81610.89</v>
@@ -5631,7 +5631,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9944109320640564</v>
+        <v>0.9999449253082275</v>
       </c>
       <c r="H12" t="n">
         <v>85495.64</v>
@@ -5654,7 +5654,7 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.9950319528579712</v>
+        <v>0.9999510645866394</v>
       </c>
       <c r="H13" t="n">
         <v>89273.59</v>
@@ -5677,7 +5677,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.995652973651886</v>
+        <v>0.9999572038650513</v>
       </c>
       <c r="H14" t="n">
         <v>94044.58</v>
@@ -5700,7 +5700,7 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.9962739944458008</v>
+        <v>0.9999632835388184</v>
       </c>
       <c r="H15" t="n">
         <v>101522.6</v>
@@ -5723,7 +5723,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.9968949556350708</v>
+        <v>0.9999694228172302</v>
       </c>
       <c r="H16" t="n">
         <v>112195.7</v>
@@ -5746,7 +5746,7 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>0.9975159764289856</v>
+        <v>0.9999755024909973</v>
       </c>
       <c r="H17" t="n">
         <v>127212.1</v>
@@ -5769,7 +5769,7 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>0.9981369972229004</v>
+        <v>0.9999816417694092</v>
       </c>
       <c r="H18" t="n">
         <v>154418.1</v>
@@ -5792,7 +5792,7 @@
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19" t="n">
-        <v>0.9987580180168152</v>
+        <v>0.999987781047821</v>
       </c>
       <c r="H19" t="n">
         <v>184542.3</v>
@@ -5815,7 +5815,7 @@
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>0.9993789792060852</v>
+        <v>0.9999938607215881</v>
       </c>
       <c r="H20" t="n">
         <v>269244.0</v>
@@ -5838,7 +5838,7 @@
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>0.9994410872459412</v>
+        <v>0.9999945163726807</v>
       </c>
       <c r="H21" t="n">
         <v>293887.0</v>
@@ -5861,7 +5861,7 @@
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>0.9995031952857971</v>
+        <v>0.9999951124191284</v>
       </c>
       <c r="H22" t="n">
         <v>327254.6</v>
@@ -5884,7 +5884,7 @@
       <c r="E23"/>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>0.9995653033256531</v>
+        <v>0.9999957084655762</v>
       </c>
       <c r="H23" t="n">
         <v>335610.2</v>
@@ -5907,7 +5907,7 @@
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>0.999627411365509</v>
+        <v>0.9999963045120239</v>
       </c>
       <c r="H24" t="n">
         <v>342220.3</v>
@@ -5930,7 +5930,7 @@
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>0.999689519405365</v>
+        <v>0.9999969601631165</v>
       </c>
       <c r="H25" t="n">
         <v>371061.2</v>
@@ -5953,7 +5953,7 @@
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" t="n">
-        <v>0.999751627445221</v>
+        <v>0.9999975562095642</v>
       </c>
       <c r="H26" t="n">
         <v>420478.3</v>
@@ -5976,7 +5976,7 @@
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27" t="n">
-        <v>0.9998136758804321</v>
+        <v>0.999998152256012</v>
       </c>
       <c r="H27" t="n">
         <v>507648.2</v>
@@ -5999,7 +5999,7 @@
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>0.9998757839202881</v>
+        <v>0.9999987483024597</v>
       </c>
       <c r="H28" t="n">
         <v>666671.7</v>
@@ -6022,7 +6022,7 @@
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>0.999937891960144</v>
+        <v>0.9999994039535522</v>
       </c>
       <c r="H29" t="n">
         <v>1071471.0</v>
@@ -6045,7 +6045,7 @@
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>0.9999440908432007</v>
+        <v>0.999999463558197</v>
       </c>
       <c r="H30" t="n">
         <v>1155125.0</v>
@@ -6068,7 +6068,7 @@
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" t="n">
-        <v>0.9999503493309021</v>
+        <v>0.9999995231628418</v>
       </c>
       <c r="H31" t="n">
         <v>1258863.0</v>
@@ -6091,7 +6091,7 @@
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>0.9999565482139587</v>
+        <v>0.9999995827674866</v>
       </c>
       <c r="H32" t="n">
         <v>1389584.0</v>
@@ -6114,7 +6114,7 @@
       <c r="E33"/>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>0.9999627470970154</v>
+        <v>0.9999996423721313</v>
       </c>
       <c r="H33" t="n">
         <v>1558692.0</v>
@@ -6137,7 +6137,7 @@
       <c r="E34"/>
       <c r="F34"/>
       <c r="G34" t="n">
-        <v>0.999968945980072</v>
+        <v>0.9999997019767761</v>
       </c>
       <c r="H34" t="n">
         <v>1786770.0</v>
@@ -6160,7 +6160,7 @@
       <c r="E35"/>
       <c r="F35"/>
       <c r="G35" t="n">
-        <v>0.9999751448631287</v>
+        <v>0.9999997615814209</v>
       </c>
       <c r="H35" t="n">
         <v>2116807.0</v>
@@ -6183,7 +6183,7 @@
       <c r="E36"/>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>0.9999813437461853</v>
+        <v>0.9999998211860657</v>
       </c>
       <c r="H36" t="n">
         <v>2639973.0</v>
@@ -6206,7 +6206,7 @@
       <c r="E37"/>
       <c r="F37"/>
       <c r="G37" t="n">
-        <v>0.9999876022338867</v>
+        <v>0.9999998807907104</v>
       </c>
       <c r="H37" t="n">
         <v>3559170.0</v>
@@ -6229,7 +6229,7 @@
       <c r="E38"/>
       <c r="F38"/>
       <c r="G38" t="n">
-        <v>0.9999938011169434</v>
+        <v>0.9999999403953552</v>
       </c>
       <c r="H38" t="n">
         <v>5616808.0</v>
@@ -6292,13 +6292,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>2.15602051E8</v>
+        <v>2.11140729E8</v>
       </c>
       <c r="F2" t="n">
-        <v>26710.699747152965</v>
+        <v>27275.08650939327</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8113627035950599</v>
+        <v>0.807376870428443</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -6321,7 +6321,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8181487011920865</v>
+        <v>0.8143062535319749</v>
       </c>
       <c r="H3" t="n">
         <v>7920.0</v>
@@ -6344,7 +6344,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8215398795069904</v>
+        <v>0.8177690861340163</v>
       </c>
       <c r="H4" t="n">
         <v>15840.0</v>
@@ -6367,7 +6367,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8399357388302396</v>
+        <v>0.836553642854951</v>
       </c>
       <c r="H5" t="n">
         <v>31680.0</v>
@@ -6390,7 +6390,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8794850054557227</v>
+        <v>0.8769385701988365</v>
       </c>
       <c r="H6" t="n">
         <v>47520.0</v>
@@ -6413,7 +6413,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9276473997921291</v>
+        <v>0.9261186173132897</v>
       </c>
       <c r="H7" t="n">
         <v>79200.0</v>
@@ -6436,7 +6436,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9510899689910649</v>
+        <v>0.9500565189390816</v>
       </c>
       <c r="H8" t="n">
         <v>110880.0</v>
@@ -6459,7 +6459,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9684821597545934</v>
+        <v>0.9678161999715366</v>
       </c>
       <c r="H9" t="n">
         <v>158400.0</v>
@@ -6482,7 +6482,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9818757382785751</v>
+        <v>0.9814927796332464</v>
       </c>
       <c r="H10" t="n">
         <v>237600.0</v>
@@ -6505,7 +6505,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.988141550657141</v>
+        <v>0.9878909862056979</v>
       </c>
       <c r="H11" t="n">
         <v>316800.0</v>
@@ -6528,7 +6528,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9937335800205351</v>
+        <v>0.9936011729882774</v>
       </c>
       <c r="H12" t="n">
         <v>475200.0</v>
@@ -6551,7 +6551,7 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.9961602962673115</v>
+        <v>0.9960791648114466</v>
       </c>
       <c r="H13" t="n">
         <v>633600.0</v>
@@ -6574,7 +6574,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.9979902232006133</v>
+        <v>0.9979477573936008</v>
       </c>
       <c r="H14" t="n">
         <v>950400.0</v>
@@ -6597,7 +6597,7 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.9987069649907923</v>
+        <v>0.9986796436607926</v>
       </c>
       <c r="H15" t="n">
         <v>1267200.0</v>
@@ -6620,7 +6620,7 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.9995010761748273</v>
+        <v>0.9994905341072304</v>
       </c>
       <c r="H16" t="n">
         <v>2534400.0</v>
@@ -6643,7 +6643,7 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>0.9997023033885702</v>
+        <v>0.9996960131742275</v>
       </c>
       <c r="H17" t="n">
         <v>3801600.0</v>
@@ -6666,7 +6666,7 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>0.9997926875009181</v>
+        <v>0.9997883070679366</v>
       </c>
       <c r="H18" t="n">
         <v>5068800.0</v>
@@ -6732,10 +6732,10 @@
         <v>1.17123344E8</v>
       </c>
       <c r="F2" t="n">
-        <v>8651.298222959465</v>
+        <v>85.67030377800782</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8613835573196411</v>
+        <v>0.9986273646354675</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -6758,7 +6758,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8746528625488281</v>
+        <v>0.9987587332725525</v>
       </c>
       <c r="H3" t="n">
         <v>2090.09</v>
@@ -6781,7 +6781,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.878832995891571</v>
+        <v>0.9988001585006714</v>
       </c>
       <c r="H4" t="n">
         <v>4181.08</v>
@@ -6804,7 +6804,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.886099636554718</v>
+        <v>0.9988721013069153</v>
       </c>
       <c r="H5" t="n">
         <v>8361.39</v>
@@ -6827,7 +6827,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8957885503768921</v>
+        <v>0.9989680647850037</v>
       </c>
       <c r="H6" t="n">
         <v>12540.95</v>
@@ -6850,7 +6850,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9359078407287598</v>
+        <v>0.9993653297424316</v>
       </c>
       <c r="H7" t="n">
         <v>20911.100000000002</v>
@@ -6873,7 +6873,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9682598114013672</v>
+        <v>0.9996857047080994</v>
       </c>
       <c r="H8" t="n">
         <v>41832.78</v>
@@ -6896,7 +6896,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9841299057006836</v>
+        <v>0.9998428225517273</v>
       </c>
       <c r="H9" t="n">
         <v>82704.38</v>
@@ -6959,13 +6959,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>1.89953924E8</v>
+        <v>1.8855232E8</v>
       </c>
       <c r="F2" t="n">
-        <v>5140.926867483243</v>
+        <v>5179.141956330583</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8672058598799991</v>
+        <v>0.8662187344075108</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -6988,7 +6988,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8812933235325004</v>
+        <v>0.8804109172456749</v>
       </c>
       <c r="H3" t="n">
         <v>2280.0</v>
@@ -7011,7 +7011,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8852669503158039</v>
+        <v>0.8844140819906114</v>
       </c>
       <c r="H4" t="n">
         <v>4560.0</v>
@@ -7034,7 +7034,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8925702793062595</v>
+        <v>0.8917717002898718</v>
       </c>
       <c r="H5" t="n">
         <v>9120.0</v>
@@ -7057,7 +7057,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.901987905235377</v>
+        <v>0.9012593321577799</v>
       </c>
       <c r="H6" t="n">
         <v>13680.0</v>
@@ -7080,7 +7080,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9394519115067084</v>
+        <v>0.9390018271851548</v>
       </c>
       <c r="H7" t="n">
         <v>22800.0</v>
@@ -7103,7 +7103,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9726906457589157</v>
+        <v>0.9724876416264727</v>
       </c>
       <c r="H8" t="n">
         <v>45600.0</v>
@@ -7126,7 +7126,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9888491432269648</v>
+        <v>0.9887662533136691</v>
       </c>
       <c r="H9" t="n">
         <v>91200.0</v>
@@ -7149,7 +7149,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9961536672440628</v>
+        <v>0.9961250755228045</v>
       </c>
       <c r="H10" t="n">
         <v>182400.0</v>
@@ -7172,7 +7172,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9989218490690406</v>
+        <v>0.9989138346322124</v>
       </c>
       <c r="H11" t="n">
         <v>364800.0</v>
@@ -7195,7 +7195,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9996494097168532</v>
+        <v>0.9996468036033712</v>
       </c>
       <c r="H12" t="n">
         <v>729600.0</v>
@@ -7258,13 +7258,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>1.91999849E8</v>
+        <v>1.90367302E8</v>
       </c>
       <c r="F2" t="n">
-        <v>6530.303415420134</v>
+        <v>6586.305823070656</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8657688788078162</v>
+        <v>0.8646177430197546</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -7287,7 +7287,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8787025556462807</v>
+        <v>0.8776623361505643</v>
       </c>
       <c r="H3" t="n">
         <v>2490.0</v>
@@ -7310,7 +7310,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8823517095578549</v>
+        <v>0.8813427843821624</v>
       </c>
       <c r="H4" t="n">
         <v>4980.0</v>
@@ -7333,7 +7333,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8894446526361591</v>
+        <v>0.8884965549388308</v>
       </c>
       <c r="H5" t="n">
         <v>9960.0</v>
@@ -7356,7 +7356,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8994125354754836</v>
+        <v>0.8985499200907937</v>
       </c>
       <c r="H6" t="n">
         <v>14940.0</v>
@@ -7379,7 +7379,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.937803878168675</v>
+        <v>0.9372704982707587</v>
       </c>
       <c r="H7" t="n">
         <v>24900.0</v>
@@ -7402,7 +7402,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9716654412577168</v>
+        <v>0.9714224504794421</v>
       </c>
       <c r="H8" t="n">
         <v>49800.0</v>
@@ -7425,7 +7425,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9883732877310752</v>
+        <v>0.9882735796717863</v>
       </c>
       <c r="H9" t="n">
         <v>99600.0</v>
@@ -7448,7 +7448,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9959690489131583</v>
+        <v>0.995934480386763</v>
       </c>
       <c r="H10" t="n">
         <v>199200.0</v>
@@ -7471,7 +7471,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9988625616054521</v>
+        <v>0.9988528071905962</v>
       </c>
       <c r="H11" t="n">
         <v>398400.0</v>
@@ -7494,7 +7494,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9996278226239647</v>
+        <v>0.9996246309148196</v>
       </c>
       <c r="H12" t="n">
         <v>796800.0</v>
@@ -7557,13 +7557,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>1.93995123E8</v>
+        <v>1.92079951E8</v>
       </c>
       <c r="F2" t="n">
-        <v>6866.849765453846</v>
+        <v>6935.317079874411</v>
       </c>
       <c r="G2" t="n">
-        <v>0.874308108250742</v>
+        <v>0.8730548718226193</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -7586,7 +7586,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8835952695573692</v>
+        <v>0.8824346326494013</v>
       </c>
       <c r="H3" t="n">
         <v>2790.0</v>
@@ -7609,7 +7609,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8863711537737987</v>
+        <v>0.8852381943808388</v>
       </c>
       <c r="H4" t="n">
         <v>5580.0</v>
@@ -7632,7 +7632,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8918845604175317</v>
+        <v>0.8908065735606107</v>
       </c>
       <c r="H5" t="n">
         <v>11160.0</v>
@@ -7655,7 +7655,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9012117588131326</v>
+        <v>0.9002267706742595</v>
       </c>
       <c r="H6" t="n">
         <v>16740.0</v>
@@ -7678,7 +7678,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9393880226566315</v>
+        <v>0.9387836786776357</v>
       </c>
       <c r="H7" t="n">
         <v>27900.0</v>
@@ -7701,7 +7701,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9725284124797302</v>
+        <v>0.9722545014601758</v>
       </c>
       <c r="H8" t="n">
         <v>55800.0</v>
@@ -7724,7 +7724,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9888216571300094</v>
+        <v>0.9887102012015819</v>
       </c>
       <c r="H9" t="n">
         <v>111600.0</v>
@@ -7747,7 +7747,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9961915125051881</v>
+        <v>0.9961535392103469</v>
       </c>
       <c r="H10" t="n">
         <v>223200.0</v>
@@ -7770,7 +7770,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9989748247434035</v>
+        <v>0.9989646030261639</v>
       </c>
       <c r="H11" t="n">
         <v>446400.0</v>
@@ -7793,7 +7793,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9996667648186187</v>
+        <v>0.9996634422298453</v>
       </c>
       <c r="H12" t="n">
         <v>892800.0</v>
@@ -7856,13 +7856,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>1.9591021E8</v>
+        <v>1.93701929E8</v>
       </c>
       <c r="F2" t="n">
-        <v>7717.327049880657</v>
+        <v>7805.307726082584</v>
       </c>
       <c r="G2" t="n">
-        <v>0.877683848126139</v>
+        <v>0.8762893941030396</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -7885,7 +7885,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8852558730859408</v>
+        <v>0.8839477432359488</v>
       </c>
       <c r="H3" t="n">
         <v>3060.0</v>
@@ -7908,7 +7908,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.887922778501437</v>
+        <v>0.8866450524609902</v>
       </c>
       <c r="H4" t="n">
         <v>6120.0</v>
@@ -7931,7 +7931,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8931914370363851</v>
+        <v>0.8919737758522787</v>
       </c>
       <c r="H5" t="n">
         <v>12240.0</v>
@@ -7954,7 +7954,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.9030334151548304</v>
+        <v>0.9019279565357349</v>
       </c>
       <c r="H6" t="n">
         <v>18360.0</v>
@@ -7977,7 +7977,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9377165539253927</v>
+        <v>0.9370064972352443</v>
       </c>
       <c r="H7" t="n">
         <v>30600.0</v>
@@ -8000,7 +8000,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9717737069446253</v>
+        <v>0.9714519156905247</v>
       </c>
       <c r="H8" t="n">
         <v>61200.0</v>
@@ -8023,7 +8023,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.988568594765939</v>
+        <v>0.9884382720834959</v>
       </c>
       <c r="H9" t="n">
         <v>122400.0</v>
@@ -8046,7 +8046,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9960793620710222</v>
+        <v>0.9960346651994364</v>
       </c>
       <c r="H10" t="n">
         <v>244800.0</v>
@@ -8069,7 +8069,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9989217560432404</v>
+        <v>0.9989094636223267</v>
       </c>
       <c r="H11" t="n">
         <v>489600.0</v>
@@ -8092,7 +8092,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9996392990441897</v>
+        <v>0.9996351869061665</v>
       </c>
       <c r="H12" t="n">
         <v>979200.0</v>
@@ -8155,13 +8155,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>1.97825297E8</v>
+        <v>1.95284734E8</v>
       </c>
       <c r="F2" t="n">
-        <v>8896.71825288871</v>
+        <v>9012.46039387303</v>
       </c>
       <c r="G2" t="n">
-        <v>0.874140540276808</v>
+        <v>0.8725031676055128</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -8184,7 +8184,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8813379665998935</v>
+        <v>0.8797942290768105</v>
       </c>
       <c r="H3" t="n">
         <v>3270.0</v>
@@ -8207,7 +8207,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8838447440824517</v>
+        <v>0.8823336185612952</v>
       </c>
       <c r="H4" t="n">
         <v>6540.0</v>
@@ -8230,7 +8230,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8887491825678897</v>
+        <v>0.8873018614962499</v>
       </c>
       <c r="H5" t="n">
         <v>13080.0</v>
@@ -8253,7 +8253,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8981195564690596</v>
+        <v>0.8967941395767269</v>
       </c>
       <c r="H6" t="n">
         <v>19620.0</v>
@@ -8276,7 +8276,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9338654247034948</v>
+        <v>0.9330050448285425</v>
       </c>
       <c r="H7" t="n">
         <v>32700.0</v>
@@ -8299,7 +8299,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9698704054011859</v>
+        <v>0.9694784334755014</v>
       </c>
       <c r="H8" t="n">
         <v>65400.0</v>
@@ -8322,7 +8322,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9877171876557325</v>
+        <v>0.9875573940152435</v>
       </c>
       <c r="H9" t="n">
         <v>130800.0</v>
@@ -8345,7 +8345,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9957372640770003</v>
+        <v>0.9956818078775169</v>
       </c>
       <c r="H10" t="n">
         <v>261600.0</v>
@@ -8368,7 +8368,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9987883602166411</v>
+        <v>0.9987725973500827</v>
       </c>
       <c r="H11" t="n">
         <v>523200.0</v>
@@ -8391,7 +8391,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9995909016630972</v>
+        <v>0.9995855794851839</v>
       </c>
       <c r="H12" t="n">
         <v>1046400.0</v>
@@ -8454,13 +8454,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>1.99688907E8</v>
+        <v>1.96876111E8</v>
       </c>
       <c r="F2" t="n">
-        <v>9660.410456064643</v>
+        <v>9798.430065204406</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8704291771199889</v>
+        <v>0.8685779810024793</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -8483,7 +8483,7 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.8773548247224369</v>
+        <v>0.8756025762820965</v>
       </c>
       <c r="H3" t="n">
         <v>3732.0</v>
@@ -8506,7 +8506,7 @@
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.8798620145684908</v>
+        <v>0.8781455866933495</v>
       </c>
       <c r="H4" t="n">
         <v>7464.0</v>
@@ -8529,7 +8529,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.8851071982681542</v>
+        <v>0.8834657090519225</v>
       </c>
       <c r="H5" t="n">
         <v>14928.0</v>
@@ -8552,7 +8552,7 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.8960505753081216</v>
+        <v>0.8945654356205767</v>
       </c>
       <c r="H6" t="n">
         <v>22392.0</v>
@@ -8575,7 +8575,7 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.9350281235201513</v>
+        <v>0.934099861409798</v>
       </c>
       <c r="H7" t="n">
         <v>37320.0</v>
@@ -8598,7 +8598,7 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.9711788497094633</v>
+        <v>0.9707670779823562</v>
       </c>
       <c r="H8" t="n">
         <v>74640.0</v>
@@ -8621,7 +8621,7 @@
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.9885613826310342</v>
+        <v>0.9883979575358435</v>
       </c>
       <c r="H9" t="n">
         <v>149280.0</v>
@@ -8644,7 +8644,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.9962103753715272</v>
+        <v>0.996156232484702</v>
       </c>
       <c r="H10" t="n">
         <v>298560.0</v>
@@ -8667,7 +8667,7 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.9989167199958684</v>
+        <v>0.9989012430258742</v>
       </c>
       <c r="H11" t="n">
         <v>597120.0</v>
@@ -8690,7 +8690,7 @@
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.9996307105832374</v>
+        <v>0.9996254344946909</v>
       </c>
       <c r="H12" t="n">
         <v>1194240.0</v>

</xml_diff>